<commit_message>
Add Planet Earth splitting code and update Budapest code
</commit_message>
<xml_diff>
--- a/MovieWithEyetracking/movies/Budapest/Code/Budapest_Exact_Splits.xlsx
+++ b/MovieWithEyetracking/movies/Budapest/Code/Budapest_Exact_Splits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmt/Movies/Bluray/Budapest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmt/Movies/Bluray/Budapest/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E087B1-4FAB-9246-87A3-20F7CA832E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E4CCA3-B91D-7749-BAB8-D3EF0D566B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24000" yWindow="9640" windowWidth="14740" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24760" yWindow="4820" windowWidth="26440" windowHeight="18340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Splits" sheetId="1" r:id="rId1"/>
@@ -896,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -907,6 +907,7 @@
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
     <col min="3" max="3" width="19.1640625" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -925,82 +926,109 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3">
         <v>5.2314814814814824E-4</v>
       </c>
       <c r="C2" s="3">
-        <v>1.3094907407407408E-2</v>
+        <v>1.1857638888888888E-2</v>
       </c>
       <c r="D2" s="3">
         <f>C2-B2</f>
-        <v>1.257175925925926E-2</v>
+        <v>1.133449074074074E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>2</v>
+        <f>A2+1</f>
+        <v>1</v>
       </c>
       <c r="B3" s="3">
         <f>C2-(5/24/60/60)+(1/30/24/60/60)</f>
-        <v>1.3037422839506175E-2</v>
+        <v>1.1800154320987655E-2</v>
       </c>
       <c r="C3" s="3">
-        <v>2.7995370370370368E-2</v>
+        <v>2.2357638888888889E-2</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D6" si="0">C3-B3</f>
-        <v>1.4957947530864194E-2</v>
+        <f t="shared" ref="D3:D5" si="0">C3-B3</f>
+        <v>1.0557484567901234E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>3</v>
+        <f>A3+1</f>
+        <v>2</v>
       </c>
       <c r="B4" s="3">
-        <f t="shared" ref="B4:B6" si="1">C3-(5/24/60/60)+(1/30/24/60/60)</f>
-        <v>2.7937885802469132E-2</v>
+        <f t="shared" ref="B4:B5" si="1">C3-(5/24/60/60)+(1/30/24/60/60)</f>
+        <v>2.2300154320987652E-2</v>
       </c>
       <c r="C4" s="3">
-        <v>4.3605706018518514E-2</v>
+        <v>3.3594907407407407E-2</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" si="0"/>
-        <v>1.5667820216049382E-2</v>
+        <v>1.1294753086419754E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>4</v>
+        <f>A4+1</f>
+        <v>3</v>
       </c>
       <c r="B5" s="3">
         <f t="shared" si="1"/>
-        <v>4.3548221450617285E-2</v>
+        <v>3.3537422839506177E-2</v>
       </c>
       <c r="C5" s="3">
-        <v>5.6108796296296302E-2</v>
+        <v>4.3605706018518514E-2</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" si="0"/>
-        <v>1.2560574845679018E-2</v>
+        <v>1.0068283179012337E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
+        <f>A5+1</f>
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" ref="B6" si="2">C5-(5/24/60/60)+(1/30/24/60/60)</f>
+        <v>4.3548221450617285E-2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5.3692129629629631E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" ref="D6" si="3">C6-B6</f>
+        <v>1.0143908179012347E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <f>A6+1</f>
         <v>5</v>
       </c>
-      <c r="B6" s="3">
-        <f t="shared" si="1"/>
-        <v>5.6051311728395073E-2</v>
-      </c>
-      <c r="C6" s="3">
-        <v>6.5162037037037032E-2</v>
-      </c>
-      <c r="D6" s="3">
-        <f t="shared" si="0"/>
-        <v>9.1107253086419593E-3</v>
-      </c>
+      <c r="B7" s="3">
+        <f t="shared" ref="B7" si="4">C6-(5/24/60/60)+(1/30/24/60/60)</f>
+        <v>5.3634645061728402E-2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>6.5173611111111113E-2</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" ref="D7" si="5">C7-B7</f>
+        <v>1.1538966049382711E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>